<commit_message>
Updated BOM to change wording for NEMA17 and to add compare of working area to PrintNC.
</commit_message>
<xml_diff>
--- a/BOM/PrintNC Mini BOM (Public).xlsx
+++ b/BOM/PrintNC Mini BOM (Public).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\PNC-Mini-CAD\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E70B6E-E9DF-4992-B7AB-EF7AB6A5BE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A6FF32E-D119-4AA6-A24C-57A86590927E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V3" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="247">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1211,6 +1211,12 @@
   <si>
     <t>Qty my built</t>
   </si>
+  <si>
+    <t>PrintNC</t>
+  </si>
+  <si>
+    <t>Delta PrintNC Mini vs. PrintNC</t>
+  </si>
 </sst>
 </file>
 
@@ -1810,7 +1816,7 @@
     <xf numFmtId="0" fontId="39" fillId="9" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="40" fillId="10" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2132,46 +2138,8 @@
     <xf numFmtId="0" fontId="34" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2212,6 +2180,48 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Berechnung" xfId="4" builtinId="22"/>
@@ -2437,9 +2447,9 @@
   </sheetPr>
   <dimension ref="A1:AB1061"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F99" sqref="F99"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2473,7 +2483,7 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="145" t="s">
+      <c r="G1" s="129" t="s">
         <v>244</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -2501,16 +2511,16 @@
       <c r="AB1" s="4"/>
     </row>
     <row r="2" spans="1:28" ht="69.599999999999994" customHeight="1">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="131" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="129"/>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
-      <c r="E2" s="129"/>
-      <c r="F2" s="129"/>
-      <c r="G2" s="129"/>
-      <c r="H2" s="129"/>
+      <c r="B2" s="132"/>
+      <c r="C2" s="132"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="132"/>
+      <c r="G2" s="132"/>
+      <c r="H2" s="132"/>
       <c r="I2" s="95"/>
       <c r="J2" s="4" t="s">
         <v>222</v>
@@ -2564,16 +2574,16 @@
       <c r="AB3" s="4"/>
     </row>
     <row r="4" spans="1:28" ht="15.6">
-      <c r="A4" s="121" t="s">
+      <c r="A4" s="133" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="118"/>
-      <c r="C4" s="118"/>
-      <c r="D4" s="118"/>
-      <c r="E4" s="118"/>
-      <c r="F4" s="118"/>
-      <c r="G4" s="118"/>
-      <c r="H4" s="119"/>
+      <c r="B4" s="134"/>
+      <c r="C4" s="134"/>
+      <c r="D4" s="134"/>
+      <c r="E4" s="134"/>
+      <c r="F4" s="134"/>
+      <c r="G4" s="134"/>
+      <c r="H4" s="135"/>
       <c r="I4" s="97"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -2653,10 +2663,10 @@
         <v>13</v>
       </c>
       <c r="E6" s="16"/>
-      <c r="F6" s="131" t="s">
+      <c r="F6" s="138" t="s">
         <v>234</v>
       </c>
-      <c r="G6" s="146">
+      <c r="G6" s="130">
         <v>1</v>
       </c>
       <c r="H6" s="115">
@@ -2696,8 +2706,8 @@
         <v>13</v>
       </c>
       <c r="E7" s="21"/>
-      <c r="F7" s="132"/>
-      <c r="G7" s="137"/>
+      <c r="F7" s="139"/>
+      <c r="G7" s="121"/>
       <c r="H7" s="44"/>
       <c r="I7" s="99"/>
       <c r="J7" s="4"/>
@@ -2733,8 +2743,8 @@
         <v>13</v>
       </c>
       <c r="E8" s="21"/>
-      <c r="F8" s="132"/>
-      <c r="G8" s="137"/>
+      <c r="F8" s="139"/>
+      <c r="G8" s="121"/>
       <c r="H8" s="44"/>
       <c r="I8" s="99"/>
       <c r="J8" s="4"/>
@@ -2771,8 +2781,8 @@
         <v>218</v>
       </c>
       <c r="E9" s="21"/>
-      <c r="F9" s="132"/>
-      <c r="G9" s="137"/>
+      <c r="F9" s="139"/>
+      <c r="G9" s="121"/>
       <c r="H9" s="44"/>
       <c r="I9" s="99"/>
       <c r="J9" s="4"/>
@@ -2809,8 +2819,8 @@
         <v>220</v>
       </c>
       <c r="E10" s="19"/>
-      <c r="F10" s="132"/>
-      <c r="G10" s="137"/>
+      <c r="F10" s="139"/>
+      <c r="G10" s="121"/>
       <c r="H10" s="44"/>
       <c r="I10" s="99"/>
       <c r="J10" s="4"/>
@@ -2839,8 +2849,8 @@
       <c r="C11" s="26"/>
       <c r="D11" s="27"/>
       <c r="E11" s="24"/>
-      <c r="F11" s="133"/>
-      <c r="G11" s="138"/>
+      <c r="F11" s="140"/>
+      <c r="G11" s="122"/>
       <c r="H11" s="37"/>
       <c r="I11" s="99"/>
       <c r="J11" s="4"/>
@@ -2921,7 +2931,7 @@
         <v>22</v>
       </c>
       <c r="E13" s="14"/>
-      <c r="F13" s="131" t="s">
+      <c r="F13" s="138" t="s">
         <v>235</v>
       </c>
       <c r="G13" s="111"/>
@@ -2960,7 +2970,7 @@
         <v>22</v>
       </c>
       <c r="E14" s="19"/>
-      <c r="F14" s="132"/>
+      <c r="F14" s="139"/>
       <c r="G14" s="112"/>
       <c r="H14" s="19"/>
       <c r="I14" s="99"/>
@@ -2998,7 +3008,7 @@
         <v>25</v>
       </c>
       <c r="E15" s="19"/>
-      <c r="F15" s="132"/>
+      <c r="F15" s="139"/>
       <c r="G15" s="112"/>
       <c r="H15" s="19"/>
       <c r="I15" s="99"/>
@@ -3028,8 +3038,8 @@
       <c r="C16" s="34"/>
       <c r="D16" s="35"/>
       <c r="E16" s="34"/>
-      <c r="F16" s="132"/>
-      <c r="G16" s="137"/>
+      <c r="F16" s="139"/>
+      <c r="G16" s="121"/>
       <c r="H16" s="37"/>
       <c r="I16" s="99"/>
       <c r="J16" s="4"/>
@@ -3110,7 +3120,7 @@
         <v>29</v>
       </c>
       <c r="E18" s="14"/>
-      <c r="F18" s="131" t="s">
+      <c r="F18" s="138" t="s">
         <v>236</v>
       </c>
       <c r="G18" s="111"/>
@@ -3150,7 +3160,7 @@
         <v>31</v>
       </c>
       <c r="E19" s="19"/>
-      <c r="F19" s="132"/>
+      <c r="F19" s="139"/>
       <c r="G19" s="112"/>
       <c r="H19" s="19"/>
       <c r="I19" s="99"/>
@@ -3303,7 +3313,7 @@
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="21"/>
-      <c r="G23" s="139"/>
+      <c r="G23" s="123"/>
       <c r="H23" s="44"/>
       <c r="I23" s="99"/>
       <c r="J23" s="4"/>
@@ -3343,7 +3353,7 @@
       <c r="F24" s="113" t="s">
         <v>237</v>
       </c>
-      <c r="G24" s="140"/>
+      <c r="G24" s="124"/>
       <c r="H24" s="44"/>
       <c r="I24" s="99"/>
       <c r="J24" s="4"/>
@@ -3373,7 +3383,7 @@
       <c r="D25" s="46"/>
       <c r="E25" s="34"/>
       <c r="F25" s="114"/>
-      <c r="G25" s="141"/>
+      <c r="G25" s="125"/>
       <c r="H25" s="37"/>
       <c r="I25" s="99"/>
       <c r="J25" s="4"/>
@@ -3441,16 +3451,16 @@
       <c r="AB26" s="4"/>
     </row>
     <row r="27" spans="1:28" ht="13.8">
-      <c r="A27" s="130" t="s">
+      <c r="A27" s="136" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="118"/>
-      <c r="C27" s="118"/>
-      <c r="D27" s="118"/>
-      <c r="E27" s="118"/>
-      <c r="F27" s="118"/>
-      <c r="G27" s="118"/>
-      <c r="H27" s="119"/>
+      <c r="B27" s="134"/>
+      <c r="C27" s="134"/>
+      <c r="D27" s="134"/>
+      <c r="E27" s="134"/>
+      <c r="F27" s="134"/>
+      <c r="G27" s="134"/>
+      <c r="H27" s="135"/>
       <c r="I27" s="99"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
@@ -3509,7 +3519,7 @@
       <c r="AB28" s="4"/>
     </row>
     <row r="29" spans="1:28" ht="52.8">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="92" t="s">
         <v>42</v>
       </c>
       <c r="B29" s="18">
@@ -3525,7 +3535,7 @@
       <c r="F29" s="110" t="s">
         <v>233</v>
       </c>
-      <c r="G29" s="146">
+      <c r="G29" s="130">
         <v>1</v>
       </c>
       <c r="H29" s="115">
@@ -3567,10 +3577,10 @@
         <v>46</v>
       </c>
       <c r="E30" s="19"/>
-      <c r="F30" s="134" t="s">
+      <c r="F30" s="118" t="s">
         <v>241</v>
       </c>
-      <c r="G30" s="146">
+      <c r="G30" s="130">
         <v>2</v>
       </c>
       <c r="H30" s="115">
@@ -3598,16 +3608,16 @@
       <c r="AB30" s="4"/>
     </row>
     <row r="31" spans="1:28" ht="13.8">
-      <c r="A31" s="130" t="s">
+      <c r="A31" s="136" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="118"/>
-      <c r="C31" s="118"/>
-      <c r="D31" s="118"/>
-      <c r="E31" s="118"/>
-      <c r="F31" s="118"/>
-      <c r="G31" s="118"/>
-      <c r="H31" s="119"/>
+      <c r="B31" s="134"/>
+      <c r="C31" s="134"/>
+      <c r="D31" s="134"/>
+      <c r="E31" s="134"/>
+      <c r="F31" s="134"/>
+      <c r="G31" s="134"/>
+      <c r="H31" s="135"/>
       <c r="I31" s="99"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
@@ -3750,7 +3760,7 @@
       <c r="D35" s="35"/>
       <c r="E35" s="24"/>
       <c r="F35" s="49"/>
-      <c r="G35" s="142"/>
+      <c r="G35" s="126"/>
       <c r="H35" s="19"/>
       <c r="I35" s="99"/>
       <c r="J35" s="4"/>
@@ -3818,16 +3828,16 @@
       <c r="AB36" s="4"/>
     </row>
     <row r="37" spans="1:28" ht="13.8">
-      <c r="A37" s="117" t="s">
+      <c r="A37" s="137" t="s">
         <v>57</v>
       </c>
-      <c r="B37" s="118"/>
-      <c r="C37" s="118"/>
-      <c r="D37" s="118"/>
-      <c r="E37" s="118"/>
-      <c r="F37" s="118"/>
-      <c r="G37" s="118"/>
-      <c r="H37" s="119"/>
+      <c r="B37" s="134"/>
+      <c r="C37" s="134"/>
+      <c r="D37" s="134"/>
+      <c r="E37" s="134"/>
+      <c r="F37" s="134"/>
+      <c r="G37" s="134"/>
+      <c r="H37" s="135"/>
       <c r="I37" s="99"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
@@ -3888,16 +3898,16 @@
       <c r="AB38" s="4"/>
     </row>
     <row r="39" spans="1:28" ht="13.8">
-      <c r="A39" s="117" t="s">
+      <c r="A39" s="137" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="118"/>
-      <c r="C39" s="118"/>
-      <c r="D39" s="118"/>
-      <c r="E39" s="118"/>
-      <c r="F39" s="118"/>
-      <c r="G39" s="118"/>
-      <c r="H39" s="119"/>
+      <c r="B39" s="134"/>
+      <c r="C39" s="134"/>
+      <c r="D39" s="134"/>
+      <c r="E39" s="134"/>
+      <c r="F39" s="134"/>
+      <c r="G39" s="134"/>
+      <c r="H39" s="135"/>
       <c r="I39" s="99"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
@@ -4070,16 +4080,16 @@
       <c r="AB43" s="4"/>
     </row>
     <row r="44" spans="1:28" ht="13.2">
-      <c r="A44" s="120" t="s">
+      <c r="A44" s="141" t="s">
         <v>67</v>
       </c>
-      <c r="B44" s="118"/>
-      <c r="C44" s="118"/>
-      <c r="D44" s="118"/>
-      <c r="E44" s="118"/>
-      <c r="F44" s="118"/>
-      <c r="G44" s="118"/>
-      <c r="H44" s="119"/>
+      <c r="B44" s="134"/>
+      <c r="C44" s="134"/>
+      <c r="D44" s="134"/>
+      <c r="E44" s="134"/>
+      <c r="F44" s="134"/>
+      <c r="G44" s="134"/>
+      <c r="H44" s="135"/>
       <c r="I44" s="99"/>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
@@ -4117,10 +4127,10 @@
       <c r="E45" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F45" s="135" t="s">
+      <c r="F45" s="119" t="s">
         <v>243</v>
       </c>
-      <c r="G45" s="146">
+      <c r="G45" s="130">
         <v>1</v>
       </c>
       <c r="H45" s="115">
@@ -4412,16 +4422,16 @@
       <c r="AB52" s="4"/>
     </row>
     <row r="53" spans="1:28" ht="13.2">
-      <c r="A53" s="120" t="s">
+      <c r="A53" s="141" t="s">
         <v>86</v>
       </c>
-      <c r="B53" s="118"/>
-      <c r="C53" s="118"/>
-      <c r="D53" s="118"/>
-      <c r="E53" s="118"/>
-      <c r="F53" s="118"/>
-      <c r="G53" s="118"/>
-      <c r="H53" s="119"/>
+      <c r="B53" s="134"/>
+      <c r="C53" s="134"/>
+      <c r="D53" s="134"/>
+      <c r="E53" s="134"/>
+      <c r="F53" s="134"/>
+      <c r="G53" s="134"/>
+      <c r="H53" s="135"/>
       <c r="I53" s="99"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
@@ -4510,16 +4520,16 @@
       <c r="AB55" s="4"/>
     </row>
     <row r="56" spans="1:28" ht="13.2">
-      <c r="A56" s="122" t="s">
+      <c r="A56" s="142" t="s">
         <v>89</v>
       </c>
-      <c r="B56" s="123"/>
-      <c r="C56" s="123"/>
-      <c r="D56" s="123"/>
-      <c r="E56" s="123"/>
-      <c r="F56" s="123"/>
-      <c r="G56" s="123"/>
-      <c r="H56" s="124"/>
+      <c r="B56" s="143"/>
+      <c r="C56" s="143"/>
+      <c r="D56" s="143"/>
+      <c r="E56" s="143"/>
+      <c r="F56" s="143"/>
+      <c r="G56" s="143"/>
+      <c r="H56" s="144"/>
       <c r="I56" s="99"/>
       <c r="J56" s="60"/>
       <c r="K56" s="60"/>
@@ -4621,7 +4631,7 @@
       <c r="D59" s="35"/>
       <c r="E59" s="37"/>
       <c r="F59" s="36"/>
-      <c r="G59" s="143"/>
+      <c r="G59" s="127"/>
       <c r="H59" s="37"/>
       <c r="I59" s="99"/>
       <c r="J59" s="4"/>
@@ -4705,16 +4715,16 @@
       <c r="AB61" s="4"/>
     </row>
     <row r="62" spans="1:28" ht="15.6">
-      <c r="A62" s="121" t="s">
+      <c r="A62" s="133" t="s">
         <v>94</v>
       </c>
-      <c r="B62" s="118"/>
-      <c r="C62" s="118"/>
-      <c r="D62" s="118"/>
-      <c r="E62" s="118"/>
-      <c r="F62" s="118"/>
-      <c r="G62" s="118"/>
-      <c r="H62" s="119"/>
+      <c r="B62" s="134"/>
+      <c r="C62" s="134"/>
+      <c r="D62" s="134"/>
+      <c r="E62" s="134"/>
+      <c r="F62" s="134"/>
+      <c r="G62" s="134"/>
+      <c r="H62" s="135"/>
       <c r="I62" s="99"/>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
@@ -5060,7 +5070,7 @@
       <c r="C71" s="67" t="s">
         <v>112</v>
       </c>
-      <c r="D71" s="125" t="s">
+      <c r="D71" s="145" t="s">
         <v>113</v>
       </c>
       <c r="E71" s="14"/>
@@ -5098,7 +5108,7 @@
       <c r="C72" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="D72" s="126"/>
+      <c r="D72" s="146"/>
       <c r="E72" s="19"/>
       <c r="F72" s="40"/>
       <c r="G72" s="40"/>
@@ -5134,7 +5144,7 @@
       <c r="C73" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="D73" s="126"/>
+      <c r="D73" s="146"/>
       <c r="E73" s="19"/>
       <c r="F73" s="40"/>
       <c r="G73" s="40"/>
@@ -5280,7 +5290,7 @@
       <c r="C77" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="D77" s="127" t="s">
+      <c r="D77" s="147" t="s">
         <v>122</v>
       </c>
       <c r="E77" s="19"/>
@@ -5322,7 +5332,7 @@
       <c r="C78" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="D78" s="126"/>
+      <c r="D78" s="146"/>
       <c r="E78" s="19"/>
       <c r="F78" s="40"/>
       <c r="G78" s="40">
@@ -5362,7 +5372,7 @@
       <c r="C79" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="D79" s="126"/>
+      <c r="D79" s="146"/>
       <c r="E79" s="19"/>
       <c r="F79" s="40"/>
       <c r="G79" s="40"/>
@@ -5398,7 +5408,7 @@
       <c r="C80" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="D80" s="126"/>
+      <c r="D80" s="146"/>
       <c r="E80" s="19"/>
       <c r="F80" s="40"/>
       <c r="G80" s="40"/>
@@ -5663,16 +5673,16 @@
       <c r="AB87" s="4"/>
     </row>
     <row r="88" spans="1:28" ht="15.6">
-      <c r="A88" s="121" t="s">
+      <c r="A88" s="133" t="s">
         <v>132</v>
       </c>
-      <c r="B88" s="118"/>
-      <c r="C88" s="118"/>
-      <c r="D88" s="118"/>
-      <c r="E88" s="118"/>
-      <c r="F88" s="118"/>
-      <c r="G88" s="118"/>
-      <c r="H88" s="119"/>
+      <c r="B88" s="134"/>
+      <c r="C88" s="134"/>
+      <c r="D88" s="134"/>
+      <c r="E88" s="134"/>
+      <c r="F88" s="134"/>
+      <c r="G88" s="134"/>
+      <c r="H88" s="135"/>
       <c r="I88" s="99"/>
       <c r="J88" s="4"/>
       <c r="K88" s="4"/>
@@ -5750,7 +5760,7 @@
         <v>135</v>
       </c>
       <c r="E90" s="14"/>
-      <c r="F90" s="135" t="s">
+      <c r="F90" s="119" t="s">
         <v>242</v>
       </c>
       <c r="G90" s="19">
@@ -6026,16 +6036,16 @@
       <c r="AB97" s="4"/>
     </row>
     <row r="98" spans="1:28" ht="15.6">
-      <c r="A98" s="121" t="s">
+      <c r="A98" s="133" t="s">
         <v>148</v>
       </c>
-      <c r="B98" s="118"/>
-      <c r="C98" s="118"/>
-      <c r="D98" s="118"/>
-      <c r="E98" s="118"/>
-      <c r="F98" s="118"/>
-      <c r="G98" s="118"/>
-      <c r="H98" s="119"/>
+      <c r="B98" s="134"/>
+      <c r="C98" s="134"/>
+      <c r="D98" s="134"/>
+      <c r="E98" s="134"/>
+      <c r="F98" s="134"/>
+      <c r="G98" s="134"/>
+      <c r="H98" s="135"/>
       <c r="I98" s="99"/>
       <c r="J98" s="4"/>
       <c r="K98" s="4"/>
@@ -6562,16 +6572,16 @@
       <c r="AB112" s="4"/>
     </row>
     <row r="113" spans="1:28" ht="15.6">
-      <c r="A113" s="121" t="s">
+      <c r="A113" s="133" t="s">
         <v>172</v>
       </c>
-      <c r="B113" s="118"/>
-      <c r="C113" s="118"/>
-      <c r="D113" s="118"/>
-      <c r="E113" s="118"/>
-      <c r="F113" s="118"/>
-      <c r="G113" s="118"/>
-      <c r="H113" s="119"/>
+      <c r="B113" s="134"/>
+      <c r="C113" s="134"/>
+      <c r="D113" s="134"/>
+      <c r="E113" s="134"/>
+      <c r="F113" s="134"/>
+      <c r="G113" s="134"/>
+      <c r="H113" s="135"/>
       <c r="I113" s="99"/>
       <c r="J113" s="4"/>
       <c r="K113" s="4"/>
@@ -6822,7 +6832,7 @@
       <c r="D120" s="7"/>
       <c r="E120" s="4"/>
       <c r="F120" s="44"/>
-      <c r="G120" s="144"/>
+      <c r="G120" s="128"/>
       <c r="H120" s="4"/>
       <c r="I120" s="99"/>
       <c r="J120" s="4"/>
@@ -6846,16 +6856,16 @@
       <c r="AB120" s="4"/>
     </row>
     <row r="121" spans="1:28" ht="15.6">
-      <c r="A121" s="121" t="s">
+      <c r="A121" s="133" t="s">
         <v>184</v>
       </c>
-      <c r="B121" s="118"/>
-      <c r="C121" s="118"/>
-      <c r="D121" s="118"/>
-      <c r="E121" s="118"/>
-      <c r="F121" s="118"/>
-      <c r="G121" s="118"/>
-      <c r="H121" s="119"/>
+      <c r="B121" s="134"/>
+      <c r="C121" s="134"/>
+      <c r="D121" s="134"/>
+      <c r="E121" s="134"/>
+      <c r="F121" s="134"/>
+      <c r="G121" s="134"/>
+      <c r="H121" s="135"/>
       <c r="I121" s="99"/>
       <c r="J121" s="4"/>
       <c r="K121" s="4"/>
@@ -7789,7 +7799,7 @@
       <c r="E147" s="4"/>
       <c r="F147" s="4"/>
       <c r="G147" s="4"/>
-      <c r="H147" s="136">
+      <c r="H147" s="120">
         <f>SUMPRODUCT(G6:G145,H6:H145)</f>
         <v>962.41</v>
       </c>
@@ -35235,14 +35245,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="A37:H37"/>
-    <mergeCell ref="F6:F11"/>
-    <mergeCell ref="F13:F16"/>
-    <mergeCell ref="F18:F19"/>
     <mergeCell ref="A39:H39"/>
     <mergeCell ref="A44:H44"/>
     <mergeCell ref="A113:H113"/>
@@ -35254,6 +35256,14 @@
     <mergeCell ref="D77:D80"/>
     <mergeCell ref="A88:H88"/>
     <mergeCell ref="A98:H98"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="A37:H37"/>
+    <mergeCell ref="F6:F11"/>
+    <mergeCell ref="F13:F16"/>
+    <mergeCell ref="F18:F19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D38" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
@@ -35298,10 +35308,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C6FCBDC-8D30-4C12-A096-C7786AC175EE}">
-  <dimension ref="B2:I27"/>
+  <dimension ref="B2:I31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
@@ -35324,9 +35334,14 @@
       <c r="C4" s="102" t="s">
         <v>226</v>
       </c>
-      <c r="D4" s="99"/>
-      <c r="E4" s="102" t="s">
+      <c r="D4" s="102" t="s">
         <v>227</v>
+      </c>
+      <c r="F4" s="148" t="s">
+        <v>245</v>
+      </c>
+      <c r="G4" s="117" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="13.8">
@@ -35337,13 +35352,16 @@
         <f>258.42+1.58</f>
         <v>260</v>
       </c>
-      <c r="D5" s="99"/>
-      <c r="E5" s="103">
-        <f>C5-C22+E22</f>
-        <v>660</v>
-      </c>
-      <c r="H5" s="104" t="s">
-        <v>228</v>
+      <c r="D5" s="103">
+        <f>C5-C22+D22</f>
+        <v>560</v>
+      </c>
+      <c r="F5">
+        <v>470</v>
+      </c>
+      <c r="G5">
+        <f>D5-F5</f>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="13.8">
@@ -35354,13 +35372,16 @@
         <f>128+173</f>
         <v>301</v>
       </c>
-      <c r="D6" s="99"/>
-      <c r="E6" s="103">
-        <f>C6-C23+E23</f>
-        <v>491</v>
-      </c>
-      <c r="H6" s="107" t="s">
-        <v>229</v>
+      <c r="D6" s="103">
+        <f>C6-C23+D23</f>
+        <v>601</v>
+      </c>
+      <c r="F6">
+        <v>510</v>
+      </c>
+      <c r="G6">
+        <f>D6-F6</f>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="2:9">
@@ -35371,7 +35392,7 @@
         <f>82.117+21.883</f>
         <v>104</v>
       </c>
-      <c r="E7" s="105">
+      <c r="D7" s="105">
         <f>82.117+21.883</f>
         <v>104</v>
       </c>
@@ -35382,9 +35403,7 @@
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
     </row>
     <row r="10" spans="2:9" ht="13.8">
       <c r="B10" s="101" t="s">
@@ -35393,9 +35412,12 @@
       <c r="C10" s="4">
         <v>450</v>
       </c>
-      <c r="E10" s="103">
-        <f>C10-C22+E22</f>
-        <v>850</v>
+      <c r="D10" s="103">
+        <f>C10-C22+D22</f>
+        <v>750</v>
+      </c>
+      <c r="F10">
+        <v>600</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="13.8">
@@ -35405,9 +35427,12 @@
       <c r="C11" s="4">
         <v>390</v>
       </c>
-      <c r="E11" s="103">
-        <f>C11-C22+E22</f>
-        <v>790</v>
+      <c r="D11" s="103">
+        <f>C11-C22+D22</f>
+        <v>690</v>
+      </c>
+      <c r="F11">
+        <v>600</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="13.8">
@@ -35417,9 +35442,12 @@
       <c r="C12" s="4">
         <v>430</v>
       </c>
-      <c r="E12" s="103">
-        <f>C12-C23+E23</f>
-        <v>620</v>
+      <c r="D12" s="103">
+        <f>C12-C23+D23</f>
+        <v>730</v>
+      </c>
+      <c r="F12">
+        <v>250</v>
       </c>
       <c r="I12" s="108"/>
     </row>
@@ -35437,7 +35465,7 @@
         <v>20</v>
       </c>
       <c r="C15" s="99"/>
-      <c r="E15" s="99"/>
+      <c r="D15" s="99"/>
       <c r="I15" s="108"/>
     </row>
     <row r="16" spans="2:9" ht="13.8">
@@ -35447,9 +35475,12 @@
       <c r="C16" s="4">
         <v>540</v>
       </c>
-      <c r="E16" s="103">
-        <f>C16-C22+E22</f>
-        <v>940</v>
+      <c r="D16" s="103">
+        <f>C16-C22+D22</f>
+        <v>840</v>
+      </c>
+      <c r="F16">
+        <v>700</v>
       </c>
       <c r="I16" s="108"/>
     </row>
@@ -35460,8 +35491,11 @@
       <c r="C17" s="4">
         <v>510</v>
       </c>
-      <c r="E17" s="103">
-        <f>C17-C23+E23</f>
+      <c r="D17" s="103">
+        <f>C17-C23+D23</f>
+        <v>810</v>
+      </c>
+      <c r="F17">
         <v>700</v>
       </c>
       <c r="I17" s="108"/>
@@ -35470,6 +35504,12 @@
       <c r="B18" s="101" t="s">
         <v>24</v>
       </c>
+      <c r="C18">
+        <v>230</v>
+      </c>
+      <c r="F18">
+        <v>300</v>
+      </c>
       <c r="I18" s="108"/>
     </row>
     <row r="19" spans="2:9">
@@ -35488,9 +35528,12 @@
       <c r="C21" s="4">
         <v>535</v>
       </c>
-      <c r="E21" s="103">
-        <f>C21-C22+E22</f>
-        <v>935</v>
+      <c r="D21" s="103">
+        <f>C21-C22+D22</f>
+        <v>835</v>
+      </c>
+      <c r="F21">
+        <v>825</v>
       </c>
       <c r="I21" s="108"/>
     </row>
@@ -35501,8 +35544,11 @@
       <c r="C22" s="4">
         <v>500</v>
       </c>
-      <c r="E22" s="106">
-        <v>900</v>
+      <c r="D22" s="106">
+        <v>800</v>
+      </c>
+      <c r="F22">
+        <v>800</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="13.8">
@@ -35512,8 +35558,11 @@
       <c r="C23" s="4">
         <v>500</v>
       </c>
-      <c r="E23" s="106">
-        <v>690</v>
+      <c r="D23" s="106">
+        <v>800</v>
+      </c>
+      <c r="F23">
+        <v>800</v>
       </c>
     </row>
     <row r="24" spans="2:9">
@@ -35534,12 +35583,25 @@
         <f>ROUNDUP((C5+C6+100+2*PI()*(55+25))/500,0)*500</f>
         <v>1500</v>
       </c>
-      <c r="E27" s="104">
-        <f>ROUNDUP((E5+E6+100+2*PI()*(55+25))/500,0)*500</f>
+      <c r="D27" s="104">
+        <f>ROUNDUP((D5+D6+100+2*PI()*(55+25))/500,0)*500</f>
         <v>2000</v>
       </c>
     </row>
+    <row r="30" spans="2:9" ht="13.8">
+      <c r="D30" s="104" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" ht="13.8">
+      <c r="D31" s="107" t="s">
+        <v>229</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{7F20E15E-7337-4C5A-A72D-7B8257B2B0CC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the PrintNC Mini BOM Excel Sheet Working Area calculation and added V47 values.
</commit_message>
<xml_diff>
--- a/BOM/PrintNC Mini BOM (Public).xlsx
+++ b/BOM/PrintNC Mini BOM (Public).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\PNC-Mini-CAD\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A6FF32E-D119-4AA6-A24C-57A86590927E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A552E661-4490-40C4-A1A0-742F596764CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="248">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1215,7 +1215,11 @@
     <t>PrintNC</t>
   </si>
   <si>
-    <t>Delta PrintNC Mini vs. PrintNC</t>
+    <t>Size Version 47
+500mm x 50mm</t>
+  </si>
+  <si>
+    <t>Delta PrintNC Mini V32 vs. PrintNC</t>
   </si>
 </sst>
 </file>
@@ -1226,7 +1230,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
   </numFmts>
-  <fonts count="49">
+  <fonts count="51">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1542,8 +1546,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1606,6 +1624,16 @@
       <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -1809,14 +1837,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="39" fillId="9" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="40" fillId="10" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="49" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="50" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2180,33 +2210,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2221,12 +2234,42 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="13" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="49" fillId="12" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="50" fillId="13" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Berechnung" xfId="4" builtinId="22"/>
     <cellStyle name="Eingabe" xfId="3" builtinId="20"/>
+    <cellStyle name="Gut" xfId="5" builtinId="26"/>
     <cellStyle name="Link" xfId="2" builtinId="8"/>
+    <cellStyle name="Schlecht" xfId="6" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Währung" xfId="1" builtinId="4"/>
   </cellStyles>
@@ -2448,8 +2491,8 @@
   <dimension ref="A1:AB1061"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
+      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2511,16 +2554,16 @@
       <c r="AB1" s="4"/>
     </row>
     <row r="2" spans="1:28" ht="69.599999999999994" customHeight="1">
-      <c r="A2" s="131" t="s">
+      <c r="A2" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="132"/>
-      <c r="C2" s="132"/>
-      <c r="D2" s="132"/>
-      <c r="E2" s="132"/>
-      <c r="F2" s="132"/>
-      <c r="G2" s="132"/>
-      <c r="H2" s="132"/>
+      <c r="B2" s="144"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="144"/>
+      <c r="H2" s="144"/>
       <c r="I2" s="95"/>
       <c r="J2" s="4" t="s">
         <v>222</v>
@@ -2574,16 +2617,16 @@
       <c r="AB3" s="4"/>
     </row>
     <row r="4" spans="1:28" ht="15.6">
-      <c r="A4" s="133" t="s">
+      <c r="A4" s="136" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="134"/>
-      <c r="C4" s="134"/>
-      <c r="D4" s="134"/>
-      <c r="E4" s="134"/>
-      <c r="F4" s="134"/>
-      <c r="G4" s="134"/>
-      <c r="H4" s="135"/>
+      <c r="B4" s="133"/>
+      <c r="C4" s="133"/>
+      <c r="D4" s="133"/>
+      <c r="E4" s="133"/>
+      <c r="F4" s="133"/>
+      <c r="G4" s="133"/>
+      <c r="H4" s="134"/>
       <c r="I4" s="97"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -2663,7 +2706,7 @@
         <v>13</v>
       </c>
       <c r="E6" s="16"/>
-      <c r="F6" s="138" t="s">
+      <c r="F6" s="146" t="s">
         <v>234</v>
       </c>
       <c r="G6" s="130">
@@ -2706,7 +2749,7 @@
         <v>13</v>
       </c>
       <c r="E7" s="21"/>
-      <c r="F7" s="139"/>
+      <c r="F7" s="147"/>
       <c r="G7" s="121"/>
       <c r="H7" s="44"/>
       <c r="I7" s="99"/>
@@ -2743,7 +2786,7 @@
         <v>13</v>
       </c>
       <c r="E8" s="21"/>
-      <c r="F8" s="139"/>
+      <c r="F8" s="147"/>
       <c r="G8" s="121"/>
       <c r="H8" s="44"/>
       <c r="I8" s="99"/>
@@ -2781,7 +2824,7 @@
         <v>218</v>
       </c>
       <c r="E9" s="21"/>
-      <c r="F9" s="139"/>
+      <c r="F9" s="147"/>
       <c r="G9" s="121"/>
       <c r="H9" s="44"/>
       <c r="I9" s="99"/>
@@ -2819,7 +2862,7 @@
         <v>220</v>
       </c>
       <c r="E10" s="19"/>
-      <c r="F10" s="139"/>
+      <c r="F10" s="147"/>
       <c r="G10" s="121"/>
       <c r="H10" s="44"/>
       <c r="I10" s="99"/>
@@ -2849,7 +2892,7 @@
       <c r="C11" s="26"/>
       <c r="D11" s="27"/>
       <c r="E11" s="24"/>
-      <c r="F11" s="140"/>
+      <c r="F11" s="148"/>
       <c r="G11" s="122"/>
       <c r="H11" s="37"/>
       <c r="I11" s="99"/>
@@ -2931,7 +2974,7 @@
         <v>22</v>
       </c>
       <c r="E13" s="14"/>
-      <c r="F13" s="138" t="s">
+      <c r="F13" s="146" t="s">
         <v>235</v>
       </c>
       <c r="G13" s="111"/>
@@ -2970,7 +3013,7 @@
         <v>22</v>
       </c>
       <c r="E14" s="19"/>
-      <c r="F14" s="139"/>
+      <c r="F14" s="147"/>
       <c r="G14" s="112"/>
       <c r="H14" s="19"/>
       <c r="I14" s="99"/>
@@ -3008,7 +3051,7 @@
         <v>25</v>
       </c>
       <c r="E15" s="19"/>
-      <c r="F15" s="139"/>
+      <c r="F15" s="147"/>
       <c r="G15" s="112"/>
       <c r="H15" s="19"/>
       <c r="I15" s="99"/>
@@ -3038,7 +3081,7 @@
       <c r="C16" s="34"/>
       <c r="D16" s="35"/>
       <c r="E16" s="34"/>
-      <c r="F16" s="139"/>
+      <c r="F16" s="147"/>
       <c r="G16" s="121"/>
       <c r="H16" s="37"/>
       <c r="I16" s="99"/>
@@ -3120,7 +3163,7 @@
         <v>29</v>
       </c>
       <c r="E18" s="14"/>
-      <c r="F18" s="138" t="s">
+      <c r="F18" s="146" t="s">
         <v>236</v>
       </c>
       <c r="G18" s="111"/>
@@ -3160,7 +3203,7 @@
         <v>31</v>
       </c>
       <c r="E19" s="19"/>
-      <c r="F19" s="139"/>
+      <c r="F19" s="147"/>
       <c r="G19" s="112"/>
       <c r="H19" s="19"/>
       <c r="I19" s="99"/>
@@ -3451,16 +3494,16 @@
       <c r="AB26" s="4"/>
     </row>
     <row r="27" spans="1:28" ht="13.8">
-      <c r="A27" s="136" t="s">
+      <c r="A27" s="145" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="134"/>
-      <c r="C27" s="134"/>
-      <c r="D27" s="134"/>
-      <c r="E27" s="134"/>
-      <c r="F27" s="134"/>
-      <c r="G27" s="134"/>
-      <c r="H27" s="135"/>
+      <c r="B27" s="133"/>
+      <c r="C27" s="133"/>
+      <c r="D27" s="133"/>
+      <c r="E27" s="133"/>
+      <c r="F27" s="133"/>
+      <c r="G27" s="133"/>
+      <c r="H27" s="134"/>
       <c r="I27" s="99"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
@@ -3608,16 +3651,16 @@
       <c r="AB30" s="4"/>
     </row>
     <row r="31" spans="1:28" ht="13.8">
-      <c r="A31" s="136" t="s">
+      <c r="A31" s="145" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="134"/>
-      <c r="C31" s="134"/>
-      <c r="D31" s="134"/>
-      <c r="E31" s="134"/>
-      <c r="F31" s="134"/>
-      <c r="G31" s="134"/>
-      <c r="H31" s="135"/>
+      <c r="B31" s="133"/>
+      <c r="C31" s="133"/>
+      <c r="D31" s="133"/>
+      <c r="E31" s="133"/>
+      <c r="F31" s="133"/>
+      <c r="G31" s="133"/>
+      <c r="H31" s="134"/>
       <c r="I31" s="99"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
@@ -3828,16 +3871,16 @@
       <c r="AB36" s="4"/>
     </row>
     <row r="37" spans="1:28" ht="13.8">
-      <c r="A37" s="137" t="s">
+      <c r="A37" s="132" t="s">
         <v>57</v>
       </c>
-      <c r="B37" s="134"/>
-      <c r="C37" s="134"/>
-      <c r="D37" s="134"/>
-      <c r="E37" s="134"/>
-      <c r="F37" s="134"/>
-      <c r="G37" s="134"/>
-      <c r="H37" s="135"/>
+      <c r="B37" s="133"/>
+      <c r="C37" s="133"/>
+      <c r="D37" s="133"/>
+      <c r="E37" s="133"/>
+      <c r="F37" s="133"/>
+      <c r="G37" s="133"/>
+      <c r="H37" s="134"/>
       <c r="I37" s="99"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
@@ -3898,16 +3941,16 @@
       <c r="AB38" s="4"/>
     </row>
     <row r="39" spans="1:28" ht="13.8">
-      <c r="A39" s="137" t="s">
+      <c r="A39" s="132" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="134"/>
-      <c r="C39" s="134"/>
-      <c r="D39" s="134"/>
-      <c r="E39" s="134"/>
-      <c r="F39" s="134"/>
-      <c r="G39" s="134"/>
-      <c r="H39" s="135"/>
+      <c r="B39" s="133"/>
+      <c r="C39" s="133"/>
+      <c r="D39" s="133"/>
+      <c r="E39" s="133"/>
+      <c r="F39" s="133"/>
+      <c r="G39" s="133"/>
+      <c r="H39" s="134"/>
       <c r="I39" s="99"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
@@ -4080,16 +4123,16 @@
       <c r="AB43" s="4"/>
     </row>
     <row r="44" spans="1:28" ht="13.2">
-      <c r="A44" s="141" t="s">
+      <c r="A44" s="135" t="s">
         <v>67</v>
       </c>
-      <c r="B44" s="134"/>
-      <c r="C44" s="134"/>
-      <c r="D44" s="134"/>
-      <c r="E44" s="134"/>
-      <c r="F44" s="134"/>
-      <c r="G44" s="134"/>
-      <c r="H44" s="135"/>
+      <c r="B44" s="133"/>
+      <c r="C44" s="133"/>
+      <c r="D44" s="133"/>
+      <c r="E44" s="133"/>
+      <c r="F44" s="133"/>
+      <c r="G44" s="133"/>
+      <c r="H44" s="134"/>
       <c r="I44" s="99"/>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
@@ -4422,16 +4465,16 @@
       <c r="AB52" s="4"/>
     </row>
     <row r="53" spans="1:28" ht="13.2">
-      <c r="A53" s="141" t="s">
+      <c r="A53" s="135" t="s">
         <v>86</v>
       </c>
-      <c r="B53" s="134"/>
-      <c r="C53" s="134"/>
-      <c r="D53" s="134"/>
-      <c r="E53" s="134"/>
-      <c r="F53" s="134"/>
-      <c r="G53" s="134"/>
-      <c r="H53" s="135"/>
+      <c r="B53" s="133"/>
+      <c r="C53" s="133"/>
+      <c r="D53" s="133"/>
+      <c r="E53" s="133"/>
+      <c r="F53" s="133"/>
+      <c r="G53" s="133"/>
+      <c r="H53" s="134"/>
       <c r="I53" s="99"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
@@ -4520,16 +4563,16 @@
       <c r="AB55" s="4"/>
     </row>
     <row r="56" spans="1:28" ht="13.2">
-      <c r="A56" s="142" t="s">
+      <c r="A56" s="137" t="s">
         <v>89</v>
       </c>
-      <c r="B56" s="143"/>
-      <c r="C56" s="143"/>
-      <c r="D56" s="143"/>
-      <c r="E56" s="143"/>
-      <c r="F56" s="143"/>
-      <c r="G56" s="143"/>
-      <c r="H56" s="144"/>
+      <c r="B56" s="138"/>
+      <c r="C56" s="138"/>
+      <c r="D56" s="138"/>
+      <c r="E56" s="138"/>
+      <c r="F56" s="138"/>
+      <c r="G56" s="138"/>
+      <c r="H56" s="139"/>
       <c r="I56" s="99"/>
       <c r="J56" s="60"/>
       <c r="K56" s="60"/>
@@ -4715,16 +4758,16 @@
       <c r="AB61" s="4"/>
     </row>
     <row r="62" spans="1:28" ht="15.6">
-      <c r="A62" s="133" t="s">
+      <c r="A62" s="136" t="s">
         <v>94</v>
       </c>
-      <c r="B62" s="134"/>
-      <c r="C62" s="134"/>
-      <c r="D62" s="134"/>
-      <c r="E62" s="134"/>
-      <c r="F62" s="134"/>
-      <c r="G62" s="134"/>
-      <c r="H62" s="135"/>
+      <c r="B62" s="133"/>
+      <c r="C62" s="133"/>
+      <c r="D62" s="133"/>
+      <c r="E62" s="133"/>
+      <c r="F62" s="133"/>
+      <c r="G62" s="133"/>
+      <c r="H62" s="134"/>
       <c r="I62" s="99"/>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
@@ -5070,7 +5113,7 @@
       <c r="C71" s="67" t="s">
         <v>112</v>
       </c>
-      <c r="D71" s="145" t="s">
+      <c r="D71" s="140" t="s">
         <v>113</v>
       </c>
       <c r="E71" s="14"/>
@@ -5108,7 +5151,7 @@
       <c r="C72" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="D72" s="146"/>
+      <c r="D72" s="141"/>
       <c r="E72" s="19"/>
       <c r="F72" s="40"/>
       <c r="G72" s="40"/>
@@ -5144,7 +5187,7 @@
       <c r="C73" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="D73" s="146"/>
+      <c r="D73" s="141"/>
       <c r="E73" s="19"/>
       <c r="F73" s="40"/>
       <c r="G73" s="40"/>
@@ -5290,7 +5333,7 @@
       <c r="C77" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="D77" s="147" t="s">
+      <c r="D77" s="142" t="s">
         <v>122</v>
       </c>
       <c r="E77" s="19"/>
@@ -5332,7 +5375,7 @@
       <c r="C78" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="D78" s="146"/>
+      <c r="D78" s="141"/>
       <c r="E78" s="19"/>
       <c r="F78" s="40"/>
       <c r="G78" s="40">
@@ -5372,7 +5415,7 @@
       <c r="C79" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="D79" s="146"/>
+      <c r="D79" s="141"/>
       <c r="E79" s="19"/>
       <c r="F79" s="40"/>
       <c r="G79" s="40"/>
@@ -5408,7 +5451,7 @@
       <c r="C80" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="D80" s="146"/>
+      <c r="D80" s="141"/>
       <c r="E80" s="19"/>
       <c r="F80" s="40"/>
       <c r="G80" s="40"/>
@@ -5673,16 +5716,16 @@
       <c r="AB87" s="4"/>
     </row>
     <row r="88" spans="1:28" ht="15.6">
-      <c r="A88" s="133" t="s">
+      <c r="A88" s="136" t="s">
         <v>132</v>
       </c>
-      <c r="B88" s="134"/>
-      <c r="C88" s="134"/>
-      <c r="D88" s="134"/>
-      <c r="E88" s="134"/>
-      <c r="F88" s="134"/>
-      <c r="G88" s="134"/>
-      <c r="H88" s="135"/>
+      <c r="B88" s="133"/>
+      <c r="C88" s="133"/>
+      <c r="D88" s="133"/>
+      <c r="E88" s="133"/>
+      <c r="F88" s="133"/>
+      <c r="G88" s="133"/>
+      <c r="H88" s="134"/>
       <c r="I88" s="99"/>
       <c r="J88" s="4"/>
       <c r="K88" s="4"/>
@@ -6036,16 +6079,16 @@
       <c r="AB97" s="4"/>
     </row>
     <row r="98" spans="1:28" ht="15.6">
-      <c r="A98" s="133" t="s">
+      <c r="A98" s="136" t="s">
         <v>148</v>
       </c>
-      <c r="B98" s="134"/>
-      <c r="C98" s="134"/>
-      <c r="D98" s="134"/>
-      <c r="E98" s="134"/>
-      <c r="F98" s="134"/>
-      <c r="G98" s="134"/>
-      <c r="H98" s="135"/>
+      <c r="B98" s="133"/>
+      <c r="C98" s="133"/>
+      <c r="D98" s="133"/>
+      <c r="E98" s="133"/>
+      <c r="F98" s="133"/>
+      <c r="G98" s="133"/>
+      <c r="H98" s="134"/>
       <c r="I98" s="99"/>
       <c r="J98" s="4"/>
       <c r="K98" s="4"/>
@@ -6572,16 +6615,16 @@
       <c r="AB112" s="4"/>
     </row>
     <row r="113" spans="1:28" ht="15.6">
-      <c r="A113" s="133" t="s">
+      <c r="A113" s="136" t="s">
         <v>172</v>
       </c>
-      <c r="B113" s="134"/>
-      <c r="C113" s="134"/>
-      <c r="D113" s="134"/>
-      <c r="E113" s="134"/>
-      <c r="F113" s="134"/>
-      <c r="G113" s="134"/>
-      <c r="H113" s="135"/>
+      <c r="B113" s="133"/>
+      <c r="C113" s="133"/>
+      <c r="D113" s="133"/>
+      <c r="E113" s="133"/>
+      <c r="F113" s="133"/>
+      <c r="G113" s="133"/>
+      <c r="H113" s="134"/>
       <c r="I113" s="99"/>
       <c r="J113" s="4"/>
       <c r="K113" s="4"/>
@@ -6856,16 +6899,16 @@
       <c r="AB120" s="4"/>
     </row>
     <row r="121" spans="1:28" ht="15.6">
-      <c r="A121" s="133" t="s">
+      <c r="A121" s="136" t="s">
         <v>184</v>
       </c>
-      <c r="B121" s="134"/>
-      <c r="C121" s="134"/>
-      <c r="D121" s="134"/>
-      <c r="E121" s="134"/>
-      <c r="F121" s="134"/>
-      <c r="G121" s="134"/>
-      <c r="H121" s="135"/>
+      <c r="B121" s="133"/>
+      <c r="C121" s="133"/>
+      <c r="D121" s="133"/>
+      <c r="E121" s="133"/>
+      <c r="F121" s="133"/>
+      <c r="G121" s="133"/>
+      <c r="H121" s="134"/>
       <c r="I121" s="99"/>
       <c r="J121" s="4"/>
       <c r="K121" s="4"/>
@@ -35245,6 +35288,14 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="A37:H37"/>
+    <mergeCell ref="F6:F11"/>
+    <mergeCell ref="F13:F16"/>
+    <mergeCell ref="F18:F19"/>
     <mergeCell ref="A39:H39"/>
     <mergeCell ref="A44:H44"/>
     <mergeCell ref="A113:H113"/>
@@ -35256,14 +35307,6 @@
     <mergeCell ref="D77:D80"/>
     <mergeCell ref="A88:H88"/>
     <mergeCell ref="A98:H98"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="A37:H37"/>
-    <mergeCell ref="F6:F11"/>
-    <mergeCell ref="F13:F16"/>
-    <mergeCell ref="F18:F19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D38" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
@@ -35307,27 +35350,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C6FCBDC-8D30-4C12-A096-C7786AC175EE}">
-  <dimension ref="B2:I31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C6FCBDC-8D30-4C12-A096-C7786AC175EE}">
+  <dimension ref="B2:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
     <col min="2" max="2" width="42.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.109375" customWidth="1"/>
+    <col min="9" max="9" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9">
-      <c r="D2" s="99"/>
-    </row>
-    <row r="3" spans="2:9">
-      <c r="D3" s="99"/>
-    </row>
-    <row r="4" spans="2:9" ht="39.6">
+    <row r="2" spans="2:10">
+      <c r="E2" s="99"/>
+    </row>
+    <row r="3" spans="2:10">
+      <c r="E3" s="99"/>
+    </row>
+    <row r="4" spans="2:10" ht="52.8">
       <c r="B4" s="100" t="s">
         <v>225</v>
       </c>
@@ -35335,16 +35378,19 @@
         <v>226</v>
       </c>
       <c r="D4" s="102" t="s">
+        <v>246</v>
+      </c>
+      <c r="E4" s="102" t="s">
         <v>227</v>
       </c>
-      <c r="F4" s="148" t="s">
+      <c r="G4" s="131" t="s">
         <v>245</v>
       </c>
-      <c r="G4" s="117" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" ht="13.8">
+      <c r="H4" s="117" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="13.8">
       <c r="B5" s="101" t="s">
         <v>230</v>
       </c>
@@ -35352,19 +35398,23 @@
         <f>258.42+1.58</f>
         <v>260</v>
       </c>
-      <c r="D5" s="103">
-        <f>C5-C22+D22</f>
+      <c r="D5" s="152">
+        <f>1.73+268.27</f>
+        <v>270</v>
+      </c>
+      <c r="E5" s="103">
+        <f>C5-C22+E22</f>
         <v>560</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>470</v>
       </c>
-      <c r="G5">
-        <f>D5-F5</f>
+      <c r="H5">
+        <f>E5-G5</f>
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="13.8">
+    <row r="6" spans="2:10" ht="13.8">
       <c r="B6" s="101" t="s">
         <v>223</v>
       </c>
@@ -35372,19 +35422,23 @@
         <f>128+173</f>
         <v>301</v>
       </c>
-      <c r="D6" s="103">
-        <f>C6-C23+D23</f>
+      <c r="D6" s="149">
+        <f>122.516+178.546</f>
+        <v>301.06200000000001</v>
+      </c>
+      <c r="E6" s="103">
+        <f>C6-C23+E23</f>
         <v>601</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>510</v>
       </c>
-      <c r="G6">
-        <f>D6-F6</f>
+      <c r="H6">
+        <f>E6-G6</f>
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:10" ht="13.8">
       <c r="B7" s="101" t="s">
         <v>224</v>
       </c>
@@ -35392,190 +35446,232 @@
         <f>82.117+21.883</f>
         <v>104</v>
       </c>
-      <c r="D7" s="105">
+      <c r="D7" s="153">
+        <f>46.975+50.825</f>
+        <v>97.800000000000011</v>
+      </c>
+      <c r="E7" s="105">
         <f>82.117+21.883</f>
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:10">
       <c r="B9" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="2:9" ht="13.8">
+      <c r="E9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="2:10" ht="13.8">
       <c r="B10" s="101" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="4">
         <v>450</v>
       </c>
-      <c r="D10" s="103">
-        <f>C10-C22+D22</f>
+      <c r="D10" s="4">
+        <v>450</v>
+      </c>
+      <c r="E10" s="103">
+        <f>C10-C22+E22</f>
         <v>750</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>600</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="13.8">
+    <row r="11" spans="2:10" ht="13.8">
       <c r="B11" s="101" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="4">
         <v>390</v>
       </c>
-      <c r="D11" s="103">
-        <f>C11-C22+D22</f>
+      <c r="D11" s="4">
+        <v>390</v>
+      </c>
+      <c r="E11" s="103">
+        <f>C11-C22+E22</f>
         <v>690</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>600</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="13.8">
+    <row r="12" spans="2:10" ht="13.8">
       <c r="B12" s="101" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="4">
         <v>430</v>
       </c>
-      <c r="D12" s="103">
-        <f>C12-C23+D23</f>
+      <c r="D12" s="4">
+        <v>430</v>
+      </c>
+      <c r="E12" s="103">
+        <f>C12-C23+E23</f>
         <v>730</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>250</v>
       </c>
-      <c r="I12" s="108"/>
-    </row>
-    <row r="13" spans="2:9">
+      <c r="J12" s="108"/>
+    </row>
+    <row r="13" spans="2:10">
       <c r="B13" s="101" t="s">
         <v>221</v>
       </c>
-      <c r="I13" s="108"/>
-    </row>
-    <row r="14" spans="2:9">
-      <c r="I14" s="108"/>
-    </row>
-    <row r="15" spans="2:9">
+      <c r="C13" s="150">
+        <v>220</v>
+      </c>
+      <c r="D13">
+        <v>220</v>
+      </c>
+      <c r="J13" s="108"/>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="J14" s="108"/>
+    </row>
+    <row r="15" spans="2:10">
       <c r="B15" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="99"/>
       <c r="D15" s="99"/>
-      <c r="I15" s="108"/>
-    </row>
-    <row r="16" spans="2:9" ht="13.8">
+      <c r="E15" s="99"/>
+      <c r="J15" s="108"/>
+    </row>
+    <row r="16" spans="2:10" ht="13.8">
       <c r="B16" s="101" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="4">
         <v>540</v>
       </c>
-      <c r="D16" s="103">
-        <f>C16-C22+D22</f>
+      <c r="D16" s="4">
+        <v>540</v>
+      </c>
+      <c r="E16" s="103">
+        <f>C16-C22+E22</f>
         <v>840</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>700</v>
       </c>
-      <c r="I16" s="108"/>
-    </row>
-    <row r="17" spans="2:9" ht="13.8">
+      <c r="J16" s="108"/>
+    </row>
+    <row r="17" spans="2:10" ht="13.8">
       <c r="B17" s="101" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="4">
         <v>510</v>
       </c>
-      <c r="D17" s="103">
-        <f>C17-C23+D23</f>
+      <c r="D17" s="4">
+        <v>510</v>
+      </c>
+      <c r="E17" s="103">
+        <f>C17-C23+E23</f>
         <v>810</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>700</v>
       </c>
-      <c r="I17" s="108"/>
-    </row>
-    <row r="18" spans="2:9">
+      <c r="J17" s="108"/>
+    </row>
+    <row r="18" spans="2:10" ht="13.8">
       <c r="B18" s="101" t="s">
         <v>24</v>
       </c>
       <c r="C18">
         <v>230</v>
       </c>
-      <c r="F18">
+      <c r="D18" s="151">
+        <v>220</v>
+      </c>
+      <c r="E18">
+        <v>230</v>
+      </c>
+      <c r="G18">
         <v>300</v>
       </c>
-      <c r="I18" s="108"/>
-    </row>
-    <row r="19" spans="2:9">
-      <c r="I19" s="108"/>
-    </row>
-    <row r="20" spans="2:9">
+      <c r="J18" s="108"/>
+    </row>
+    <row r="19" spans="2:10">
+      <c r="J19" s="108"/>
+    </row>
+    <row r="20" spans="2:10">
       <c r="B20" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="I20" s="108"/>
-    </row>
-    <row r="21" spans="2:9" ht="13.8">
+      <c r="J20" s="108"/>
+    </row>
+    <row r="21" spans="2:10" ht="13.8">
       <c r="B21" s="101" t="s">
         <v>120</v>
       </c>
       <c r="C21" s="4">
         <v>535</v>
       </c>
-      <c r="D21" s="103">
-        <f>C21-C22+D22</f>
+      <c r="D21" s="4">
+        <v>535</v>
+      </c>
+      <c r="E21" s="103">
+        <f>C21-C22+E22</f>
         <v>835</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>825</v>
       </c>
-      <c r="I21" s="108"/>
-    </row>
-    <row r="22" spans="2:9" ht="13.8">
+      <c r="J21" s="108"/>
+    </row>
+    <row r="22" spans="2:10" ht="13.8">
       <c r="B22" s="101" t="s">
         <v>123</v>
       </c>
       <c r="C22" s="4">
         <v>500</v>
       </c>
-      <c r="D22" s="106">
+      <c r="D22" s="4">
+        <v>500</v>
+      </c>
+      <c r="E22" s="106">
         <v>800</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>800</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="13.8">
+    <row r="23" spans="2:10" ht="13.8">
       <c r="B23" s="101" t="s">
         <v>124</v>
       </c>
       <c r="C23" s="4">
         <v>500</v>
       </c>
-      <c r="D23" s="106">
+      <c r="D23" s="4">
+        <v>500</v>
+      </c>
+      <c r="E23" s="106">
         <v>800</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>800</v>
       </c>
     </row>
-    <row r="24" spans="2:9">
+    <row r="24" spans="2:10">
       <c r="B24" s="101" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="2:9">
+    <row r="26" spans="2:10">
       <c r="B26" s="8" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="27" spans="2:9" ht="13.8">
+    <row r="27" spans="2:10" ht="13.8">
       <c r="B27" s="101" t="s">
         <v>239</v>
       </c>
@@ -35583,25 +35679,26 @@
         <f>ROUNDUP((C5+C6+100+2*PI()*(55+25))/500,0)*500</f>
         <v>1500</v>
       </c>
-      <c r="D27" s="104">
-        <f>ROUNDUP((D5+D6+100+2*PI()*(55+25))/500,0)*500</f>
+      <c r="E27" s="104">
+        <f>ROUNDUP((E5+E6+100+2*PI()*(55+25))/500,0)*500</f>
         <v>2000</v>
       </c>
     </row>
-    <row r="30" spans="2:9" ht="13.8">
-      <c r="D30" s="104" t="s">
+    <row r="30" spans="2:10" ht="13.8">
+      <c r="E30" s="104" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="31" spans="2:9" ht="13.8">
-      <c r="D31" s="107" t="s">
+    <row r="31" spans="2:10" ht="13.8">
+      <c r="E31" s="107" t="s">
         <v>229</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1" xr:uid="{7F20E15E-7337-4C5A-A72D-7B8257B2B0CC}"/>
+    <hyperlink ref="G4" r:id="rId1" xr:uid="{7F20E15E-7337-4C5A-A72D-7B8257B2B0CC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>